<commit_message>
correct typo in codebook, update associated graphic
</commit_message>
<xml_diff>
--- a/resources/noaaSSTCodebook.xlsx
+++ b/resources/noaaSSTCodebook.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,15 +65,6 @@
     <t>Nino34SSTA</t>
   </si>
   <si>
-    <t>Anomaly or deviation from the 1980 - 2010 average for sea surface temperature taken at the Niño 3.4 observation point (5°North-5°South)(170-120°West</t>
-  </si>
-  <si>
-    <t>Anomaly or deviation from the 1980 - 2010 average for sea surface temperature taken at the Niño 3 observation point (5°North-5°South)(150°West-90°West)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anomaly or deviation from the 1980 - 2010 average for sea surface temperature taken at the Niño 1+2  observation point (0-10°South)(90°West-80°West) </t>
-  </si>
-  <si>
     <t>Date on which a weekly sea surface temperature measurement was taken</t>
   </si>
   <si>
@@ -83,9 +74,6 @@
     <t>Nino4SSTA</t>
   </si>
   <si>
-    <t>Anomaly or deviation from the 1980 - 2010 average for sea surface temperature taken at the Niño 4 observation point (5°North-5°South)</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -114,6 +102,18 @@
   </si>
   <si>
     <t>Measurements based on Optimum Interpolation (OI) Sea Surface Temperature (SST) V2 Methodology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anomaly or deviation from the 1981 - 2010 average for sea surface temperature taken at the Niño 1+2  observation point (0-10°South)(90°West-80°West) </t>
+  </si>
+  <si>
+    <t>Anomaly or deviation from the 1981 - 2010 average for sea surface temperature taken at the Niño 3 observation point (5°North-5°South)(150°West-90°West)</t>
+  </si>
+  <si>
+    <t>Anomaly or deviation from the 1981 - 2010 average for sea surface temperature taken at the Niño 3.4 observation point (5°North-5°South)(170-120°West</t>
+  </si>
+  <si>
+    <t>Anomaly or deviation from the 1981 - 2010 average for sea surface temperature taken at the Niño 4 observation point (5°North-5°South)</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
   <dimension ref="B2:F15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,10 +521,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>2</v>
@@ -535,16 +535,16 @@
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>23</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="38" x14ac:dyDescent="0.25">
@@ -561,7 +561,7 @@
         <v>29.2</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="57" x14ac:dyDescent="0.25">
@@ -578,7 +578,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="38" x14ac:dyDescent="0.25">
@@ -595,7 +595,7 @@
         <v>29.4</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="57" x14ac:dyDescent="0.25">
@@ -612,7 +612,7 @@
         <v>3.7</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="38" x14ac:dyDescent="0.25">
@@ -629,7 +629,7 @@
         <v>29.4</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="57" x14ac:dyDescent="0.25">
@@ -646,12 +646,12 @@
         <v>2.8</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="38" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>6</v>
@@ -663,12 +663,12 @@
         <v>30</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="57" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>6</v>
@@ -680,7 +680,7 @@
         <v>1.3</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="19" x14ac:dyDescent="0.25">
@@ -692,7 +692,7 @@
     </row>
     <row r="15" spans="2:6" ht="19" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>

</xml_diff>

<commit_message>
minor edits to article, adjust codebook
</commit_message>
<xml_diff>
--- a/resources/noaaSSTCodebook.xlsx
+++ b/resources/noaaSSTCodebook.xlsx
@@ -92,28 +92,28 @@
     <t xml:space="preserve">Sea surface temperature in degrees Celsius taken at the Niño 1+2  observation point (0-10°South)(90°West-80°West) </t>
   </si>
   <si>
-    <t>Sea surface temperature in degrees Celsius taken at the Niño 3 observation point (5°North-5°South)(150°West-90°West)</t>
-  </si>
-  <si>
-    <t>Sea surface temperature in degrees Celsius taken at the Niño 3.4 observation point (5°North-5°South)(170-120°West</t>
-  </si>
-  <si>
-    <t>Sea surface temperature in degrees Celsius taken at the Niño 4 observation point (5°North-5°South)</t>
-  </si>
-  <si>
     <t>Measurements based on Optimum Interpolation (OI) Sea Surface Temperature (SST) V2 Methodology</t>
   </si>
   <si>
-    <t xml:space="preserve">Anomaly or deviation from the 1981 - 2010 average for sea surface temperature taken at the Niño 1+2  observation point (0-10°South)(90°West-80°West) </t>
-  </si>
-  <si>
-    <t>Anomaly or deviation from the 1981 - 2010 average for sea surface temperature taken at the Niño 3 observation point (5°North-5°South)(150°West-90°West)</t>
-  </si>
-  <si>
-    <t>Anomaly or deviation from the 1981 - 2010 average for sea surface temperature taken at the Niño 3.4 observation point (5°North-5°South)(170-120°West</t>
-  </si>
-  <si>
-    <t>Anomaly or deviation from the 1981 - 2010 average for sea surface temperature taken at the Niño 4 observation point (5°North-5°South)</t>
+    <t xml:space="preserve">Anomaly or deviation from the 1981 - 2010 average for sea surface temperature taken at the Niño 1+2  observation area (0-10°South)(90°West-80°West) </t>
+  </si>
+  <si>
+    <t>Sea surface temperature in degrees Celsius taken at the Niño 3 observation area (5°North-5°South)(150°West-90°West)</t>
+  </si>
+  <si>
+    <t>Anomaly or deviation from the 1981 - 2010 average for sea surface temperature taken at the Niño 3 observation area (5°North-5°South)(150°West-90°West)</t>
+  </si>
+  <si>
+    <t>Sea surface temperature in degrees Celsius taken at the Niño 3.4 observation area (5°North-5°South)(170-120°West</t>
+  </si>
+  <si>
+    <t>Anomaly or deviation from the 1981 - 2010 average for sea surface temperature taken at the Niño 3.4 observation area (5°North-5°South)(170-120°West</t>
+  </si>
+  <si>
+    <t>Sea surface temperature in degrees Celsius taken at the Niño 4 observation area (5°North-5°South)</t>
+  </si>
+  <si>
+    <t>Anomaly or deviation from the 1981 - 2010 average for sea surface temperature taken at the Niño 4 observation area (5°North-5°South)</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
   <dimension ref="B2:F15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,7 +578,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="38" x14ac:dyDescent="0.25">
@@ -595,7 +595,7 @@
         <v>29.4</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="57" x14ac:dyDescent="0.25">
@@ -612,7 +612,7 @@
         <v>3.7</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="38" x14ac:dyDescent="0.25">
@@ -629,7 +629,7 @@
         <v>29.4</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="57" x14ac:dyDescent="0.25">
@@ -646,7 +646,7 @@
         <v>2.8</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="38" x14ac:dyDescent="0.25">
@@ -663,7 +663,7 @@
         <v>30</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="57" x14ac:dyDescent="0.25">
@@ -692,7 +692,7 @@
     </row>
     <row r="15" spans="2:6" ht="19" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>

</xml_diff>